<commit_message>
i broke sth ig? layout doesn't change anymore
</commit_message>
<xml_diff>
--- a/ClassLibrary/TestdatenDA.xlsx
+++ b/ClassLibrary/TestdatenDA.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="8_{3A6D875F-8CAB-465A-A86A-528EE459A441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27DB4DE3-79E2-4024-9E7A-74D79DFC5B9B}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{1A81A998-B639-4902-988B-734D1BD5FDEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1A81A998-B639-4902-988B-734D1BD5FDEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
SCHL: Update Exel download
</commit_message>
<xml_diff>
--- a/ClassLibrary/TestdatenDA.xlsx
+++ b/ClassLibrary/TestdatenDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htlvbat-my.sharepoint.com/personal/l_schiemer_htlvb_at/Documents/5AHWII/FriendsOfAward/ClassLibrary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{3A6D875F-8CAB-465A-A86A-528EE459A441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27DB4DE3-79E2-4024-9E7A-74D79DFC5B9B}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{3A6D875F-8CAB-465A-A86A-528EE459A441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2A93C89-6E7F-4B9D-AB91-7C5A93EEB3C1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1A81A998-B639-4902-988B-734D1BD5FDEE}"/>
   </bookViews>
@@ -36,36 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Nr</t>
   </si>
   <si>
-    <t>AbteilungKürzel</t>
-  </si>
-  <si>
     <t>Titel</t>
   </si>
   <si>
     <t>Autor:innen</t>
-  </si>
-  <si>
-    <t>MB</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>WII</t>
-  </si>
-  <si>
-    <t>WIE</t>
-  </si>
-  <si>
-    <t>GT</t>
-  </si>
-  <si>
-    <t>WI</t>
   </si>
   <si>
     <t>HalloWorld1</t>
@@ -499,21 +478,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90408C46-D83E-4C0E-93E0-B8765CB5D44B}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.90625" style="2"/>
-    <col min="2" max="2" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,81 +501,63 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -605,66 +565,51 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>